<commit_message>
1NF - oprava struktury
</commit_message>
<xml_diff>
--- a/src/BachelorThesis.1NF.DB/1NF_popis_vyznam_tabulek.xlsx
+++ b/src/BachelorThesis.1NF.DB/1NF_popis_vyznam_tabulek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\DVGithub\BachelorThesis\src\BachelorThesis.1NF.DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4823409E-03F2-4B52-B902-D752690CB520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7A32E2-CF78-492C-9087-656B59FBDCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>

</xml_diff>